<commit_message>
increased settling time before reading MUX output
</commit_message>
<xml_diff>
--- a/Hardware/wemos_wireless_sensor/misc/Taratura ADC.xlsx
+++ b/Hardware/wemos_wireless_sensor/misc/Taratura ADC.xlsx
@@ -1,38 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utente\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{A3C4C126-E1DD-4368-81F9-3263EE0133EF}"/>
+    <workbookView windowWidth="9575" windowHeight="8604"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6">
+  <si>
+    <t>Wemos w/ gain=1</t>
+  </si>
   <si>
     <t>Tester</t>
   </si>
   <si>
-    <t>gain=1</t>
-  </si>
-  <si>
-    <t>gain=1,0564</t>
+    <t>Wemos w/ gain</t>
   </si>
   <si>
     <t>errore</t>
@@ -40,27 +30,27 @@
   <si>
     <t>classe</t>
   </si>
+  <si>
+    <t>gain</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000000"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="0.000000"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -68,19 +58,356 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -88,39 +415,321 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
-    <cellStyle name="Percentuale" xfId="1" builtinId="5"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="it-IT"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -132,6 +741,33 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr defTabSz="914400">
+              <a:defRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="it-IT" altLang="en-US"/>
+              <a:t>Tester vs. ADC</a:t>
+            </a:r>
+            <a:endParaRPr lang="it-IT" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -140,26 +776,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -194,6 +810,9 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:trendline>
             <c:spPr>
               <a:ln w="19050" cap="rnd">
@@ -211,8 +830,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="4.0537839020122486E-2"/>
-                  <c:y val="-0.16708333333333333"/>
+                  <c:x val="0.0405378390201225"/>
+                  <c:y val="-0.167083333333333"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -228,7 +847,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="tx1">
                           <a:lumMod val="65000"/>
@@ -240,7 +859,6 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="it-IT"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -252,10 +870,10 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2.1874999999999999E-2</c:v>
+                  <c:v>0.021875</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.41249999999999998</c:v>
+                  <c:v>0.409375</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.734375</c:v>
@@ -264,16 +882,16 @@
                   <c:v>1.09375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.4125000000000001</c:v>
+                  <c:v>1.4125</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.6875</c:v>
+                  <c:v>1.684375</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.11876</c:v>
+                  <c:v>2.115625</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.5437500000000002</c:v>
+                  <c:v>2.540625</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -288,35 +906,30 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.41699999999999998</c:v>
+                  <c:v>0.419</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.76900000000000002</c:v>
+                  <c:v>0.77</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.161</c:v>
+                  <c:v>1.162</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.502</c:v>
+                  <c:v>1.503</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.79</c:v>
+                  <c:v>1.802</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.25</c:v>
+                  <c:v>2.261</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.67</c:v>
+                  <c:v>2.685</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-12A6-4527-A7E5-FE5492C51D26}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -372,7 +985,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -384,7 +997,6 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="365960768"/>
@@ -434,7 +1046,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -446,7 +1058,6 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="365959128"/>
@@ -485,9 +1096,8 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr lang="en-US"/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1055,7 +1665,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -1069,20 +1679,14 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>61912</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame macro="">
+    <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Grafico 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{431B8172-E0B4-4325-9A02-1ECCC2CEBF3B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Grafico 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
+        <a:off x="247650" y="1821815"/>
+        <a:ext cx="5518785" cy="2628900"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1138,7 +1742,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1171,26 +1775,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1223,23 +1810,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1381,34 +1951,30 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8716D18-B00D-4E86-8BD0-D240ABE85B11}">
-  <dimension ref="A1:E28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="6"/>
   <cols>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6666666666667" customWidth="1"/>
+    <col min="3" max="3" width="15.4444444444444" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -1419,295 +1985,310 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>2.1874999999999999E-2</v>
-      </c>
-      <c r="B2" s="4">
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="2">
+        <v>0.021875</v>
+      </c>
+      <c r="B2" s="3">
         <v>0</v>
       </c>
-      <c r="C2" s="3">
-        <v>2.3109000000000001E-2</v>
-      </c>
-      <c r="D2" s="2" t="e">
+      <c r="C2" s="2">
+        <f>A2*$G$2</f>
+        <v>0.0232421875</v>
+      </c>
+      <c r="D2" s="4" t="e">
         <f>C2/B2-1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="4">
         <f>(C2-B2)/3.2</f>
-        <v>7.2215624999999997E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>0.41249999999999998</v>
-      </c>
-      <c r="B3" s="4">
-        <v>0.41699999999999998</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0.43246400000000002</v>
-      </c>
-      <c r="D3" s="2">
-        <f t="shared" ref="D3:D9" si="0">C3/B3-1</f>
-        <v>3.7083932853717139E-2</v>
-      </c>
-      <c r="E3" s="2">
-        <f t="shared" ref="E3:E9" si="1">(C3-B3)/3.2</f>
-        <v>4.8325000000000104E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+        <v>0.00726318359375</v>
+      </c>
+      <c r="G2">
+        <v>1.0625</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2">
+        <v>0.409375</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.419</v>
+      </c>
+      <c r="C3" s="2">
+        <f t="shared" ref="C3:C9" si="0">A3*$G$2</f>
+        <v>0.4349609375</v>
+      </c>
+      <c r="D3" s="4">
+        <f t="shared" ref="D3:D9" si="1">C3/B3-1</f>
+        <v>0.038092929594272</v>
+      </c>
+      <c r="E3" s="4">
+        <f t="shared" ref="E3:E9" si="2">(C3-B3)/3.2</f>
+        <v>0.00498779296875</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2">
         <v>0.734375</v>
       </c>
-      <c r="B4" s="4">
-        <v>0.76900000000000002</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0.77579399999999998</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="B4" s="3">
+        <v>0.77</v>
+      </c>
+      <c r="C4" s="2">
         <f t="shared" si="0"/>
-        <v>8.8348504551365448E-3</v>
-      </c>
-      <c r="E4" s="2">
+        <v>0.7802734375</v>
+      </c>
+      <c r="D4" s="4">
         <f t="shared" si="1"/>
-        <v>2.1231249999999896E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+        <v>0.0133421266233766</v>
+      </c>
+      <c r="E4" s="4">
+        <f t="shared" si="2"/>
+        <v>0.00321044921874999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2">
         <v>1.09375</v>
       </c>
-      <c r="B5" s="4">
-        <v>1.161</v>
-      </c>
-      <c r="C5" s="3">
-        <v>1.155437</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="B5" s="3">
+        <v>1.162</v>
+      </c>
+      <c r="C5" s="2">
         <f t="shared" si="0"/>
-        <v>-4.7915590008613673E-3</v>
-      </c>
-      <c r="E5" s="2">
+        <v>1.162109375</v>
+      </c>
+      <c r="D5" s="4">
         <f t="shared" si="1"/>
-        <v>-1.7384374999999952E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>1.4125000000000001</v>
-      </c>
-      <c r="B6" s="4">
-        <v>1.502</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1.492165</v>
-      </c>
-      <c r="D6" s="2">
+        <v>9.41265060241392e-5</v>
+      </c>
+      <c r="E5" s="4">
+        <f t="shared" si="2"/>
+        <v>3.41796875000244e-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2">
+        <v>1.4125</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1.503</v>
+      </c>
+      <c r="C6" s="2">
         <f t="shared" si="0"/>
-        <v>-6.5479360852197521E-3</v>
-      </c>
-      <c r="E6" s="2">
+        <v>1.50078125</v>
+      </c>
+      <c r="D6" s="4">
         <f t="shared" si="1"/>
-        <v>-3.0734375000000119E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>1.6875</v>
-      </c>
-      <c r="B7" s="4">
-        <v>1.79</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1.782675</v>
-      </c>
-      <c r="D7" s="2">
+        <v>-0.00147621423819011</v>
+      </c>
+      <c r="E6" s="4">
+        <f t="shared" si="2"/>
+        <v>-0.000693359374999911</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2">
+        <v>1.684375</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1.802</v>
+      </c>
+      <c r="C7" s="2">
         <f t="shared" si="0"/>
-        <v>-4.0921787709496948E-3</v>
-      </c>
-      <c r="E7" s="2">
+        <v>1.7896484375</v>
+      </c>
+      <c r="D7" s="4">
         <f t="shared" si="1"/>
-        <v>-2.2890625000000081E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>2.11876</v>
-      </c>
-      <c r="B8" s="4">
-        <v>2.25</v>
-      </c>
-      <c r="C8" s="3">
-        <v>2.2382469999999999</v>
-      </c>
-      <c r="D8" s="2">
+        <v>-0.00685436320754729</v>
+      </c>
+      <c r="E7" s="4">
+        <f t="shared" si="2"/>
+        <v>-0.00385986328125004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2">
+        <v>2.115625</v>
+      </c>
+      <c r="B8" s="3">
+        <v>2.261</v>
+      </c>
+      <c r="C8" s="2">
         <f t="shared" si="0"/>
-        <v>-5.2235555555556479E-3</v>
-      </c>
-      <c r="E8" s="2">
+        <v>2.2478515625</v>
+      </c>
+      <c r="D8" s="4">
         <f t="shared" si="1"/>
-        <v>-3.6728125000000389E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>2.5437500000000002</v>
-      </c>
-      <c r="B9" s="4">
-        <v>2.67</v>
-      </c>
-      <c r="C9" s="3">
-        <v>2.687217</v>
-      </c>
-      <c r="D9" s="2">
+        <v>-0.00581531954887216</v>
+      </c>
+      <c r="E8" s="4">
+        <f t="shared" si="2"/>
+        <v>-0.00410888671874998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2">
+        <v>2.540625</v>
+      </c>
+      <c r="B9" s="3">
+        <v>2.685</v>
+      </c>
+      <c r="C9" s="2">
         <f t="shared" si="0"/>
-        <v>6.4483146067415564E-3</v>
-      </c>
-      <c r="E9" s="2">
+        <v>2.6994140625</v>
+      </c>
+      <c r="D9" s="4">
         <f t="shared" si="1"/>
-        <v>5.3803125000000118E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
+        <v>0.00536836592178758</v>
+      </c>
+      <c r="E9" s="4">
+        <f t="shared" si="2"/>
+        <v>0.00450439453124993</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>